<commit_message>
Small tweaks to new file
</commit_message>
<xml_diff>
--- a/data/pottedgrapes2017/pottedgrapephen_2017.xlsx
+++ b/data/pottedgrapes2017/pottedgrapephen_2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="5360" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2400" yWindow="780" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>RowNum</t>
   </si>
@@ -141,7 +141,7 @@
     <t>Flowbuds</t>
   </si>
   <si>
-    <t>Does the plant have any flower buds?</t>
+    <t>Does the plant have any flower bud (not open)?</t>
   </si>
 </sst>
 </file>
@@ -149,8 +149,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -206,8 +206,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -225,21 +229,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,11 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -581,7 +589,7 @@
     <col min="1" max="1" width="13" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -601,13 +609,16 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="5">
         <v>42897</v>
       </c>
@@ -630,6 +641,9 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -646,10 +660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -753,6 +767,9 @@
       <c r="B16" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>